<commit_message>
Update BConvert configuration Excel file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fis02\AI研究中心\02临时文件\张皓\提资转换\转EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心项目\05.电力\提资转换\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="强电" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="278">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1253,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2948,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4124,9 +4124,6 @@
       <c r="B50" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D50" s="1" t="s">
         <v>222</v>
       </c>
@@ -4148,7 +4145,7 @@
         <v>220</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>222</v>
@@ -4171,7 +4168,7 @@
         <v>220</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>222</v>
@@ -4194,7 +4191,7 @@
         <v>220</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>222</v>
@@ -4217,7 +4214,7 @@
         <v>220</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>222</v>
@@ -4240,7 +4237,7 @@
         <v>220</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>222</v>
@@ -4263,7 +4260,7 @@
         <v>220</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>222</v>
@@ -4286,7 +4283,7 @@
         <v>220</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>222</v>
@@ -4309,7 +4306,7 @@
         <v>220</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>222</v>
@@ -4332,7 +4329,7 @@
         <v>220</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>222</v>
@@ -4355,7 +4352,7 @@
         <v>220</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>222</v>
@@ -4370,21 +4367,21 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>267</v>
+        <v>222</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -4393,7 +4390,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>234</v>
       </c>
@@ -4401,25 +4398,22 @@
         <v>235</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="F62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="63" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>234</v>
       </c>
@@ -4427,19 +4421,22 @@
         <v>235</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>271</v>
+        <v>239</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -4450,22 +4447,19 @@
         <v>235</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -4476,19 +4470,22 @@
         <v>235</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -4499,45 +4496,45 @@
         <v>235</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F67" s="1">
         <v>1</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H66" s="3" t="s">
+      <c r="G67" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A67" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F67" s="1">
-        <v>0</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -4548,21 +4545,44 @@
         <v>251</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F69" s="1">
         <v>1</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H68" s="3" t="s">
+      <c r="G69" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H69" s="3" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BConvert configuration file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心项目\05.电力\提资转换\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心项目\01.通用需求\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="280">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -905,6 +905,14 @@
   <si>
     <t>内含图块</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C0浓度探测器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C02浓度探测器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1251,9 +1259,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2409,7 +2419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>108</v>
       </c>
@@ -2432,7 +2442,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>110</v>
       </c>
@@ -2455,7 +2465,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
@@ -2478,7 +2488,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>117</v>
       </c>
@@ -2501,7 +2511,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>117</v>
       </c>
@@ -2524,7 +2534,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>117</v>
       </c>
@@ -2547,7 +2557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>117</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>117</v>
       </c>
@@ -2593,7 +2603,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>123</v>
       </c>
@@ -2616,7 +2626,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>123</v>
       </c>
@@ -2639,7 +2649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>123</v>
       </c>
@@ -2647,140 +2657,134 @@
         <v>124</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F59" s="1">
-        <v>0</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A60" s="1" t="s">
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F60" s="1">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F61" s="1">
-        <v>0</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A62" s="1" t="s">
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="C64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F62" s="1">
-        <v>0</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A63" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" s="1">
-        <v>1</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A64" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2791,13 +2795,13 @@
         <v>146</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
@@ -2806,7 +2810,7 @@
         <v>12</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2817,13 +2821,13 @@
         <v>146</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F66" s="1">
         <v>1</v>
@@ -2832,24 +2836,24 @@
         <v>12</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
@@ -2858,24 +2862,24 @@
         <v>12</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F68" s="1">
         <v>1</v>
@@ -2884,7 +2888,7 @@
         <v>12</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2895,13 +2899,13 @@
         <v>160</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F69" s="1">
         <v>1</v>
@@ -2910,7 +2914,7 @@
         <v>12</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2921,13 +2925,13 @@
         <v>160</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F70" s="1">
         <v>1</v>
@@ -2936,13 +2940,65 @@
         <v>12</v>
       </c>
       <c r="H70" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="3" t="s">
         <v>264</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2950,7 +3006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement block convert duct cneter line extraction engine
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心项目\09.数据联通\提资转换\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\刘潘\提资转换\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1450,20 +1450,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="5" customWidth="1"/>
-    <col min="9" max="10" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" style="5" customWidth="1"/>
+    <col min="1" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="7" width="10.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="5" customWidth="1"/>
+    <col min="9" max="10" width="15.625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="15.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1537,7 +1535,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1573,7 +1571,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1609,7 +1607,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1645,7 +1643,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1681,7 +1679,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +1715,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1753,7 +1751,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1789,7 +1787,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1825,7 +1823,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1861,7 +1859,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1897,7 +1895,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1933,7 +1931,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1969,7 +1967,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2005,7 +2003,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2041,7 +2039,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2077,7 +2075,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -2113,7 +2111,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -2149,7 +2147,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -2185,7 +2183,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2221,7 +2219,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2257,7 +2255,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -2329,7 +2327,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -2365,7 +2363,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -2401,7 +2399,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -2437,7 +2435,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -2473,7 +2471,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -2509,7 +2507,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -2545,7 +2543,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
@@ -2581,7 +2579,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -2617,7 +2615,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -2689,7 +2687,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
@@ -2725,7 +2723,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
@@ -2761,7 +2759,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -2797,7 +2795,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
@@ -2833,7 +2831,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>280</v>
       </c>
@@ -2869,7 +2867,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -2905,7 +2903,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>87</v>
       </c>
@@ -2941,7 +2939,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -2977,7 +2975,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>282</v>
       </c>
@@ -3012,7 +3010,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>286</v>
       </c>
@@ -3047,7 +3045,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>284</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
@@ -3117,7 +3115,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>96</v>
       </c>
@@ -3152,7 +3150,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
@@ -3187,7 +3185,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>100</v>
       </c>
@@ -3222,7 +3220,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
@@ -3257,7 +3255,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>104</v>
       </c>
@@ -3292,7 +3290,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>106</v>
       </c>
@@ -3327,7 +3325,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
@@ -3362,7 +3360,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>110</v>
       </c>
@@ -3397,7 +3395,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>110</v>
       </c>
@@ -3432,7 +3430,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>117</v>
       </c>
@@ -3467,7 +3465,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
@@ -3502,7 +3500,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
@@ -3537,7 +3535,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -3572,7 +3570,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
@@ -3607,7 +3605,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>123</v>
       </c>
@@ -3642,7 +3640,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>123</v>
       </c>
@@ -3677,7 +3675,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>123</v>
       </c>
@@ -3712,7 +3710,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>123</v>
       </c>
@@ -3747,7 +3745,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>123</v>
       </c>
@@ -3782,7 +3780,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>134</v>
       </c>
@@ -3817,7 +3815,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>139</v>
       </c>
@@ -3852,7 +3850,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>143</v>
       </c>
@@ -3887,7 +3885,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
@@ -3923,7 +3921,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>145</v>
       </c>
@@ -3959,7 +3957,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
@@ -3995,7 +3993,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
@@ -4031,7 +4029,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>159</v>
       </c>
@@ -4067,7 +4065,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>159</v>
       </c>
@@ -4103,7 +4101,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>159</v>
       </c>
@@ -4139,7 +4137,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>159</v>
       </c>
@@ -4184,23 +4182,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="10.625" style="1" customWidth="1"/>
+    <col min="8" max="10" width="15.625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4238,7 +4234,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -4273,7 +4269,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>110</v>
       </c>
@@ -4308,7 +4304,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>110</v>
       </c>
@@ -4343,7 +4339,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -4378,7 +4374,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>110</v>
       </c>
@@ -4413,7 +4409,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
@@ -4448,7 +4444,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>110</v>
       </c>
@@ -4483,7 +4479,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>110</v>
       </c>
@@ -4518,7 +4514,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>110</v>
       </c>
@@ -4553,7 +4549,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -4588,7 +4584,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
@@ -4623,7 +4619,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>110</v>
       </c>
@@ -4658,7 +4654,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
@@ -4693,7 +4689,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -4728,7 +4724,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>110</v>
       </c>
@@ -4763,7 +4759,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -4798,7 +4794,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -4833,7 +4829,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>110</v>
       </c>
@@ -4868,7 +4864,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>110</v>
       </c>
@@ -4903,7 +4899,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>110</v>
       </c>
@@ -4938,7 +4934,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>110</v>
       </c>
@@ -4973,7 +4969,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>110</v>
       </c>
@@ -5008,7 +5004,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>110</v>
       </c>
@@ -5043,7 +5039,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>110</v>
       </c>
@@ -5078,7 +5074,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>110</v>
       </c>
@@ -5113,7 +5109,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>110</v>
       </c>
@@ -5148,7 +5144,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>110</v>
       </c>
@@ -5183,7 +5179,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -5218,7 +5214,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
@@ -5253,7 +5249,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -5288,7 +5284,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>110</v>
       </c>
@@ -5323,7 +5319,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
@@ -5358,7 +5354,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>110</v>
       </c>
@@ -5393,7 +5389,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>117</v>
       </c>
@@ -5428,7 +5424,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
@@ -5463,7 +5459,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>117</v>
       </c>
@@ -5498,7 +5494,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
@@ -5533,7 +5529,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>117</v>
       </c>
@@ -5568,7 +5564,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -5603,7 +5599,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -5638,7 +5634,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>117</v>
       </c>
@@ -5673,7 +5669,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>195</v>
       </c>
@@ -5711,7 +5707,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>195</v>
       </c>
@@ -5749,7 +5745,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>195</v>
       </c>
@@ -5787,7 +5783,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>195</v>
       </c>
@@ -5825,7 +5821,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>203</v>
       </c>
@@ -5863,7 +5859,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>203</v>
       </c>
@@ -5901,7 +5897,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>203</v>
       </c>
@@ -5939,7 +5935,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="72" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>203</v>
       </c>
@@ -5977,7 +5973,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>211</v>
       </c>
@@ -6012,7 +6008,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>211</v>
       </c>
@@ -6047,7 +6043,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>219</v>
       </c>
@@ -6077,7 +6073,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>219</v>
       </c>
@@ -6110,7 +6106,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>219</v>
       </c>
@@ -6143,7 +6139,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>219</v>
       </c>
@@ -6176,7 +6172,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>219</v>
       </c>
@@ -6209,7 +6205,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>219</v>
       </c>
@@ -6242,7 +6238,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>219</v>
       </c>
@@ -6275,7 +6271,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>219</v>
       </c>
@@ -6308,7 +6304,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>219</v>
       </c>
@@ -6341,7 +6337,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -6374,7 +6370,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>219</v>
       </c>
@@ -6407,7 +6403,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>219</v>
       </c>
@@ -6440,7 +6436,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>234</v>
       </c>
@@ -6475,7 +6471,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="54" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>234</v>
       </c>
@@ -6513,7 +6509,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>234</v>
       </c>
@@ -6548,7 +6544,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>234</v>
       </c>
@@ -6586,7 +6582,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>234</v>
       </c>
@@ -6621,7 +6617,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>234</v>
       </c>
@@ -6659,7 +6655,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>250</v>
       </c>
@@ -6694,7 +6690,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>250</v>
       </c>
@@ -6731,34 +6727,6 @@
       <c r="L72" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K73" s="2"/>
-      <c r="L73" s="3"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K74" s="2"/>
-      <c r="L74" s="3"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K75" s="2"/>
-      <c r="L75" s="3"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K76" s="2"/>
-      <c r="L76" s="3"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K77" s="2"/>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K78" s="2"/>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K79" s="2"/>
-      <c r="L79" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Update BConvert configuration file 增加了一个给排水的新图例
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI研究中心项目\09.数据联通\提资转换\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fis\AI研究中心\02临时文件\张皓\提资转换\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="328">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1095,6 +1095,14 @@
   </si>
   <si>
     <t>电/手动排烟阀(电机、反馈，就地手动、常闭) BEEC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>室内消火栓平面带留洞</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>块:室内消火栓平面带留洞</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4184,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6047,12 +6055,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>220</v>
+    <row r="53" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>222</v>
@@ -6071,7 +6079,7 @@
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>313</v>
@@ -6084,9 +6092,6 @@
       <c r="B54" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D54" s="1" t="s">
         <v>222</v>
       </c>
@@ -6118,7 +6123,7 @@
         <v>220</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>222</v>
@@ -6151,7 +6156,7 @@
         <v>220</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>222</v>
@@ -6184,7 +6189,7 @@
         <v>220</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>222</v>
@@ -6217,7 +6222,7 @@
         <v>220</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>222</v>
@@ -6250,7 +6255,7 @@
         <v>220</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>222</v>
@@ -6283,7 +6288,7 @@
         <v>220</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>222</v>
@@ -6316,7 +6321,7 @@
         <v>220</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>222</v>
@@ -6349,7 +6354,7 @@
         <v>220</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>222</v>
@@ -6382,7 +6387,7 @@
         <v>220</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>222</v>
@@ -6415,7 +6420,7 @@
         <v>220</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>222</v>
@@ -6440,21 +6445,21 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>267</v>
+        <v>222</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -6463,19 +6468,17 @@
         <v>115</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="J65" s="4">
-        <v>0</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="J65" s="4"/>
       <c r="K65" s="3" t="s">
         <v>308</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>234</v>
       </c>
@@ -6483,22 +6486,19 @@
         <v>235</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="F66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>317</v>
@@ -6513,7 +6513,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>234</v>
       </c>
@@ -6521,19 +6521,22 @@
         <v>235</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>271</v>
+        <v>239</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="F67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="I67" s="3" t="s">
         <v>317</v>
@@ -6556,22 +6559,19 @@
         <v>235</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>317</v>
@@ -6594,19 +6594,22 @@
         <v>235</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>317</v>
@@ -6621,7 +6624,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>234</v>
       </c>
@@ -6629,22 +6632,19 @@
         <v>235</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="F70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>317</v>
@@ -6659,27 +6659,30 @@
         <v>314</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>275</v>
+        <v>248</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="F71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>317</v>
@@ -6691,7 +6694,7 @@
         <v>308</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
@@ -6702,22 +6705,19 @@
         <v>251</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="F72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>317</v>
@@ -6732,9 +6732,43 @@
         <v>315</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K73" s="2"/>
-      <c r="L73" s="3"/>
+    <row r="73" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J73" s="4">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K74" s="2"/>
@@ -6759,6 +6793,10 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K79" s="2"/>
       <c r="L79" s="3"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K80" s="2"/>
+      <c r="L80" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Update the confign file (#2595)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\Git\ThMEPEngine\AutoLoader\Contents\Support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fis\AI研究中心\02临时文件\张皓\模板文件\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="304">
   <si>
     <t>源块名</t>
   </si>
@@ -999,6 +999,42 @@
   <si>
     <t>TextCenter</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HL3-2A混流风机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动射流灭火装置平面</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷洒型自动射流灭火装置</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷射型自动射流灭火装置</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷射型自动射流灭火装置接管</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷洒型自动射流灭火装置接管</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动消防炮平面</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动消防炮</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动消防炮接管</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1352,9 +1388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M89"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2704,7 +2742,7 @@
     </row>
     <row r="40" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>295</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>245</v>
@@ -2738,7 +2776,7 @@
     </row>
     <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>245</v>
@@ -2772,13 +2810,13 @@
     </row>
     <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>165</v>
+        <v>245</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>6</v>
@@ -2806,27 +2844,28 @@
     </row>
     <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0</v>
+        <v>294</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>293</v>
+        <v>207</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="1">
         <v>0</v>
       </c>
+      <c r="J43" s="2"/>
       <c r="K43" s="2">
         <v>0</v>
       </c>
@@ -2834,12 +2873,12 @@
         <v>139</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>136</v>
+      <c r="A44" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>207</v>
@@ -2854,7 +2893,7 @@
         <v>13</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="1">
@@ -2867,12 +2906,12 @@
         <v>139</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>135</v>
+      <c r="A45" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>207</v>
@@ -2900,15 +2939,15 @@
         <v>139</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="D46" s="3">
         <v>0</v>
@@ -2933,15 +2972,15 @@
         <v>139</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="D47" s="3">
         <v>0</v>
@@ -2966,15 +3005,15 @@
         <v>139</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="D48" s="3">
         <v>0</v>
@@ -2999,12 +3038,12 @@
         <v>139</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>245</v>
@@ -3032,12 +3071,12 @@
         <v>139</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>245</v>
@@ -3070,7 +3109,7 @@
     </row>
     <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>245</v>
@@ -3098,12 +3137,12 @@
         <v>139</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>245</v>
@@ -3136,7 +3175,7 @@
     </row>
     <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>245</v>
@@ -3168,18 +3207,20 @@
       </c>
     </row>
     <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>167</v>
+      <c r="A54" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
-        <v>180</v>
+        <v>245</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>207</v>
@@ -3195,19 +3236,19 @@
         <v>139</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>7</v>
@@ -3231,14 +3272,14 @@
     </row>
     <row r="56" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>7</v>
@@ -3262,14 +3303,14 @@
     </row>
     <row r="57" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>7</v>
@@ -3288,19 +3329,19 @@
         <v>139</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>7</v>
@@ -3324,14 +3365,14 @@
     </row>
     <row r="59" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>7</v>
@@ -3355,14 +3396,14 @@
     </row>
     <row r="60" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>7</v>
@@ -3381,19 +3422,19 @@
         <v>139</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>7</v>
@@ -3412,19 +3453,19 @@
         <v>139</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>7</v>
@@ -3443,19 +3484,19 @@
         <v>139</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>7</v>
@@ -3474,19 +3515,19 @@
         <v>139</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>7</v>
@@ -3510,14 +3551,14 @@
     </row>
     <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>7</v>
@@ -3541,14 +3582,14 @@
     </row>
     <row r="66" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>7</v>
@@ -3570,24 +3611,19 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>246</v>
+    <row r="67" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D67" s="3">
-        <v>0</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>22</v>
+        <v>207</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>207</v>
@@ -3603,7 +3639,7 @@
         <v>139</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
@@ -3611,10 +3647,10 @@
         <v>21</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D68" s="3">
         <v>0</v>
@@ -3642,12 +3678,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>25</v>
+        <v>247</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>285</v>
@@ -3678,12 +3714,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>285</v>
@@ -3714,12 +3750,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="72" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>285</v>
@@ -3750,12 +3786,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>285</v>
@@ -3787,8 +3823,8 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="72" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>213</v>
+      <c r="A73" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>28</v>
@@ -3822,21 +3858,21 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>29</v>
+    <row r="74" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="D74" s="3">
         <v>0</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>23</v>
@@ -3855,7 +3891,7 @@
         <v>139</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
@@ -3863,7 +3899,7 @@
         <v>29</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>245</v>
@@ -3872,7 +3908,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>23</v>
@@ -3891,7 +3927,7 @@
         <v>139</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
@@ -3899,7 +3935,7 @@
         <v>29</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>131</v>
+        <v>32</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>245</v>
@@ -3935,7 +3971,7 @@
         <v>29</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>245</v>
@@ -3944,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>23</v>
@@ -3963,15 +3999,15 @@
         <v>139</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>132</v>
+      <c r="B78" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>245</v>
@@ -4004,10 +4040,10 @@
     </row>
     <row r="79" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>245</v>
@@ -4016,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>23</v>
@@ -4035,12 +4071,15 @@
         <v>139</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>245</v>
@@ -4049,10 +4088,10 @@
         <v>0</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>207</v>
@@ -4062,18 +4101,18 @@
         <v>0</v>
       </c>
       <c r="K80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>245</v>
@@ -4101,22 +4140,21 @@
         <v>152</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D82" s="3"/>
+        <v>245</v>
+      </c>
+      <c r="D82" s="3">
+        <v>0</v>
+      </c>
       <c r="E82" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>7</v>
@@ -4126,19 +4164,16 @@
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2">
         <v>1</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="K82" s="2">
-        <v>0</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>152</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
@@ -4146,14 +4181,14 @@
         <v>42</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>7</v>
@@ -4166,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K83" s="2">
         <v>0</v>
@@ -4183,14 +4218,14 @@
         <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>7</v>
@@ -4203,7 +4238,7 @@
         <v>1</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K84" s="2">
         <v>0</v>
@@ -4220,14 +4255,14 @@
         <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>7</v>
@@ -4240,7 +4275,7 @@
         <v>1</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K85" s="2">
         <v>0</v>
@@ -4254,17 +4289,17 @@
     </row>
     <row r="86" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>7</v>
@@ -4277,7 +4312,7 @@
         <v>1</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K86" s="2">
         <v>0</v>
@@ -4294,14 +4329,14 @@
         <v>51</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>7</v>
@@ -4314,7 +4349,7 @@
         <v>1</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K87" s="2">
         <v>0</v>
@@ -4331,14 +4366,14 @@
         <v>51</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>7</v>
@@ -4351,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K88" s="2">
         <v>0</v>
@@ -4368,14 +4403,14 @@
         <v>51</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>7</v>
@@ -4388,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K89" s="2">
         <v>0</v>
@@ -4397,6 +4432,43 @@
         <v>152</v>
       </c>
       <c r="M89" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H90" s="3"/>
+      <c r="I90" s="1">
+        <v>1</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K90" s="2">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M90" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4409,7 +4481,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8073,33 +8145,240 @@
         <v>164</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L102" s="2"/>
-      <c r="M102" s="3"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L103" s="2"/>
-      <c r="M103" s="3"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L104" s="2"/>
-      <c r="M104" s="3"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L105" s="2"/>
-      <c r="M105" s="3"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L106" s="2"/>
-      <c r="M106" s="3"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L107" s="2"/>
-      <c r="M107" s="3"/>
+    <row r="102" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D102" s="4"/>
+      <c r="E102" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H102" s="4"/>
+      <c r="I102" s="1">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
+        <v>0</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H103" s="4">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1">
+        <v>1</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H104" s="4"/>
+      <c r="I104" s="1">
+        <v>0</v>
+      </c>
+      <c r="K104" s="1">
+        <v>0</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M104" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H105" s="4"/>
+      <c r="I105" s="1">
+        <v>1</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K105" s="1">
+        <v>0</v>
+      </c>
+      <c r="L105" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M105" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H106" s="4"/>
+      <c r="I106" s="1">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1">
+        <v>0</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M106" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H107" s="4"/>
+      <c r="I107" s="1">
+        <v>1</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K107" s="1">
+        <v>0</v>
+      </c>
+      <c r="L107" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L108" s="2"/>
       <c r="M108" s="3"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L109" s="2"/>
+      <c r="M109" s="3"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L110" s="2"/>
+      <c r="M110" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Support convert the manual actuator in TZZH (#2687)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/提资转换配置表.xlsx
+++ b/AutoLoader/Contents/Support/提资转换配置表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-228" windowWidth="30936" windowHeight="16896" activeTab="1"/>
+    <workbookView xWindow="30615" yWindow="-225" windowWidth="30930" windowHeight="16890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="强电" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="306">
   <si>
     <t>源块名</t>
   </si>
@@ -1035,6 +1035,14 @@
   <si>
     <t>自动消防炮接管</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>手动执行机构</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>手动执行机构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1391,23 +1399,23 @@
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="A76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="15.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.625" style="5" customWidth="1"/>
     <col min="11" max="11" width="12" style="5" customWidth="1"/>
-    <col min="12" max="13" width="15.6640625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="15.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1456,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1490,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>209</v>
       </c>
@@ -1516,7 +1524,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>208</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>210</v>
       </c>
@@ -1584,7 +1592,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>211</v>
       </c>
@@ -1618,7 +1626,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>212</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>214</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>215</v>
       </c>
@@ -1720,7 +1728,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>216</v>
       </c>
@@ -1754,7 +1762,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>217</v>
       </c>
@@ -1788,7 +1796,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>218</v>
       </c>
@@ -1822,7 +1830,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>219</v>
       </c>
@@ -1856,7 +1864,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>220</v>
       </c>
@@ -1890,7 +1898,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>221</v>
       </c>
@@ -1924,7 +1932,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>222</v>
       </c>
@@ -1958,7 +1966,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>223</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>224</v>
       </c>
@@ -2026,7 +2034,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>225</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>226</v>
       </c>
@@ -2094,7 +2102,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>227</v>
       </c>
@@ -2128,7 +2136,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>228</v>
       </c>
@@ -2162,7 +2170,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>229</v>
       </c>
@@ -2196,7 +2204,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>230</v>
       </c>
@@ -2230,7 +2238,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>231</v>
       </c>
@@ -2264,7 +2272,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>244</v>
       </c>
@@ -2298,7 +2306,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>232</v>
       </c>
@@ -2332,7 +2340,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>233</v>
       </c>
@@ -2366,7 +2374,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>234</v>
       </c>
@@ -2400,7 +2408,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>235</v>
       </c>
@@ -2434,7 +2442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>236</v>
       </c>
@@ -2468,7 +2476,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>237</v>
       </c>
@@ -2502,7 +2510,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>238</v>
       </c>
@@ -2536,7 +2544,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>239</v>
       </c>
@@ -2570,7 +2578,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>240</v>
       </c>
@@ -2604,7 +2612,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>241</v>
       </c>
@@ -2638,7 +2646,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>242</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>243</v>
       </c>
@@ -2706,7 +2714,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>133</v>
       </c>
@@ -2740,7 +2748,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>295</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -2808,7 +2816,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -2842,7 +2850,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -2876,7 +2884,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>134</v>
       </c>
@@ -2909,7 +2917,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>136</v>
       </c>
@@ -2942,7 +2950,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
@@ -2975,7 +2983,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -3008,7 +3016,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>14</v>
       </c>
@@ -3041,7 +3049,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>15</v>
       </c>
@@ -3074,7 +3082,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
@@ -3107,7 +3115,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -3140,7 +3148,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>18</v>
       </c>
@@ -3173,7 +3181,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>19</v>
       </c>
@@ -3206,7 +3214,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -3239,7 +3247,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>167</v>
       </c>
@@ -3270,7 +3278,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>168</v>
       </c>
@@ -3301,7 +3309,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>169</v>
       </c>
@@ -3332,7 +3340,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>170</v>
       </c>
@@ -3363,7 +3371,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>173</v>
       </c>
@@ -3394,7 +3402,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>188</v>
       </c>
@@ -3425,7 +3433,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
         <v>171</v>
       </c>
@@ -3456,7 +3464,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
         <v>172</v>
       </c>
@@ -3487,7 +3495,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>174</v>
       </c>
@@ -3518,7 +3526,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>191</v>
       </c>
@@ -3549,7 +3557,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>192</v>
       </c>
@@ -3580,7 +3588,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>193</v>
       </c>
@@ -3611,7 +3619,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>194</v>
       </c>
@@ -3642,7 +3650,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>21</v>
       </c>
@@ -3678,7 +3686,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>21</v>
       </c>
@@ -3714,7 +3722,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
@@ -3750,7 +3758,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>24</v>
       </c>
@@ -3786,7 +3794,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
@@ -3822,7 +3830,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>24</v>
       </c>
@@ -3858,7 +3866,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
         <v>213</v>
       </c>
@@ -3894,7 +3902,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>29</v>
       </c>
@@ -3930,7 +3938,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>29</v>
       </c>
@@ -3966,7 +3974,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>29</v>
       </c>
@@ -4002,7 +4010,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>29</v>
       </c>
@@ -4038,7 +4046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>29</v>
       </c>
@@ -4074,7 +4082,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>36</v>
       </c>
@@ -4110,7 +4118,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>39</v>
       </c>
@@ -4143,7 +4151,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>41</v>
       </c>
@@ -4176,7 +4184,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
@@ -4213,7 +4221,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>42</v>
       </c>
@@ -4250,7 +4258,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>42</v>
       </c>
@@ -4287,7 +4295,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>42</v>
       </c>
@@ -4324,7 +4332,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>51</v>
       </c>
@@ -4361,7 +4369,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>51</v>
       </c>
@@ -4398,7 +4406,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>51</v>
       </c>
@@ -4435,7 +4443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>51</v>
       </c>
@@ -4483,22 +4491,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" style="1" customWidth="1"/>
-    <col min="12" max="13" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="15.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4539,7 +4549,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -4575,7 +4585,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -4611,7 +4621,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -4647,7 +4657,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -4683,7 +4693,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -4719,7 +4729,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -4755,7 +4765,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -4791,7 +4801,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -4827,7 +4837,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -4863,7 +4873,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -4899,7 +4909,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -4935,7 +4945,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -4971,7 +4981,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -5007,7 +5017,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -5043,7 +5053,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -5079,7 +5089,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -5115,7 +5125,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -5151,7 +5161,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -5187,7 +5197,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -5223,7 +5233,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -5259,7 +5269,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -5295,7 +5305,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -5331,7 +5341,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -5367,7 +5377,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -5403,7 +5413,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -5439,7 +5449,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -5475,7 +5485,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -5511,7 +5521,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -5547,7 +5557,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -5583,7 +5593,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -5619,7 +5629,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -5655,7 +5665,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -5691,7 +5701,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -5727,7 +5737,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -5763,7 +5773,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
@@ -5799,7 +5809,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -5835,7 +5845,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -5871,7 +5881,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -5907,7 +5917,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -5943,7 +5953,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -5979,7 +5989,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -6015,7 +6025,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -6051,7 +6061,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -6087,7 +6097,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -6123,7 +6133,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -6159,7 +6169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -6195,7 +6205,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -6231,7 +6241,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -6267,7 +6277,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -6303,7 +6313,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
@@ -6339,7 +6349,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -6375,7 +6385,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
@@ -6411,7 +6421,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>21</v>
       </c>
@@ -6447,7 +6457,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
@@ -6483,7 +6493,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
@@ -6519,7 +6529,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -6555,7 +6565,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>21</v>
       </c>
@@ -6591,7 +6601,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
@@ -6627,7 +6637,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>21</v>
       </c>
@@ -6663,7 +6673,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
@@ -6699,7 +6709,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>21</v>
       </c>
@@ -6735,7 +6745,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>24</v>
       </c>
@@ -6771,7 +6781,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>24</v>
       </c>
@@ -6807,7 +6817,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
@@ -6843,7 +6853,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>24</v>
       </c>
@@ -6879,7 +6889,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
@@ -6915,7 +6925,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
@@ -6951,7 +6961,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -6987,7 +6997,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
@@ -7023,7 +7033,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -7062,7 +7072,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
@@ -7101,7 +7111,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>67</v>
       </c>
@@ -7140,7 +7150,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
@@ -7179,7 +7189,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -7218,7 +7228,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
@@ -7257,7 +7267,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -7296,7 +7306,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="72" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>73</v>
       </c>
@@ -7335,7 +7345,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
@@ -7371,7 +7381,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -7407,7 +7417,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>166</v>
       </c>
@@ -7438,7 +7448,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -7469,7 +7479,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -7503,7 +7513,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
@@ -7537,7 +7547,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -7571,7 +7581,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -7605,7 +7615,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
@@ -7639,7 +7649,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -7673,7 +7683,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>84</v>
       </c>
@@ -7707,7 +7717,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>84</v>
       </c>
@@ -7741,7 +7751,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>84</v>
       </c>
@@ -7775,7 +7785,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>84</v>
       </c>
@@ -7809,7 +7819,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>84</v>
       </c>
@@ -7843,7 +7853,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>97</v>
       </c>
@@ -7879,7 +7889,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
@@ -7920,7 +7930,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>97</v>
       </c>
@@ -7956,7 +7966,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>97</v>
       </c>
@@ -7995,7 +8005,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -8031,7 +8041,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -8070,7 +8080,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>110</v>
       </c>
@@ -8106,7 +8116,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>110</v>
       </c>
@@ -8145,7 +8155,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
         <v>296</v>
       </c>
@@ -8179,7 +8189,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
         <v>296</v>
       </c>
@@ -8218,7 +8228,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
         <v>296</v>
       </c>
@@ -8254,7 +8264,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
         <v>296</v>
       </c>
@@ -8293,7 +8303,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>301</v>
       </c>
@@ -8329,7 +8339,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>301</v>
       </c>
@@ -8368,15 +8378,48 @@
         <v>164</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L108" s="2"/>
-      <c r="M108" s="3"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+      <c r="A108" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D108" s="3">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H108" s="3"/>
+      <c r="I108" s="1">
+        <v>0</v>
+      </c>
+      <c r="J108" s="5"/>
+      <c r="K108" s="2">
+        <v>0</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M108" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.15">
       <c r="L109" s="2"/>
       <c r="M109" s="3"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.15">
       <c r="L110" s="2"/>
       <c r="M110" s="3"/>
     </row>

</xml_diff>